<commit_message>
Upgrade to id_diary and use DB
</commit_message>
<xml_diff>
--- a/excel_angelo.xlsx
+++ b/excel_angelo.xlsx
@@ -16,7 +16,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd h:mm:ss"/>
+    <numFmt numFmtId="165" formatCode="YYYY-MM-DD HH:MM:SS"/>
+  </numFmts>
   <fonts count="2">
     <font>
       <name val="Calibri"/>
@@ -55,11 +58,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -425,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,156 +440,275 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>univoc_id</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>id_diary</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>date start</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>date and</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>do</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>repeat</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>25</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>3541791985364674716</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>298367824096100995597</t>
-        </is>
-      </c>
       <c r="C2" t="inlineStr">
         <is>
+          <t>65592250285068942839</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
           <t>Daily event</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="E2" t="inlineStr">
         <is>
           <t>My first daily event modify</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>2024-08-15 15:00:00</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>2024-08-15 15:06:00</t>
-        </is>
-      </c>
-      <c r="G2" t="b">
+      <c r="F2" s="2" t="n">
+        <v>45519.625</v>
+      </c>
+      <c r="G2" s="2" t="n">
+        <v>45519.625</v>
+      </c>
+      <c r="H2" t="n">
         <v>1</v>
       </c>
-      <c r="H2" t="b">
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>67522624675213491256</t>
-        </is>
+      <c r="A3" t="n">
+        <v>54</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>298367824096100995597</t>
+          <t>6115568889517910016</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
+          <t>65592250285068942839</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
           <t>Monthly Event</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="E3" t="inlineStr">
         <is>
           <t>My first event monthly modify</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>2024-07-01 00:00:00</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>2024-07-31 00:00:00</t>
-        </is>
-      </c>
-      <c r="G3" t="b">
+      <c r="F3" s="2" t="n">
+        <v>45474</v>
+      </c>
+      <c r="G3" s="2" t="n">
+        <v>45474</v>
+      </c>
+      <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="H3" t="b">
+      <c r="I3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>310392366125733185</t>
-        </is>
+      <c r="A4" t="n">
+        <v>55</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>298367824096100995597</t>
+          <t>774462689499478238</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>65592250285068942839</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
           <t>Period event</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
+      <c r="E4" t="inlineStr">
         <is>
           <t>My first event period modify</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" s="2" t="n">
+        <v>45139.41666666666</v>
+      </c>
+      <c r="G4" s="2" t="n">
+        <v>45139.41666666666</v>
+      </c>
+      <c r="H4" t="n">
+        <v>1</v>
+      </c>
+      <c r="I4" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr"/>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>40764073562277591648</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>65592250285068942839</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>Daily event2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>My first daily event modify2</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>2024-08-15 15:00:00</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>2024-08-15 15:06:00</t>
+        </is>
+      </c>
+      <c r="H5" t="b">
+        <v>1</v>
+      </c>
+      <c r="I5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr"/>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>4225836343232735037</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>65592250285068942839</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Monthly Event2</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>My first event monthly modify2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>2024-07-01 00:00:00</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>2024-07-31 00:00:00</t>
+        </is>
+      </c>
+      <c r="H6" t="b">
+        <v>1</v>
+      </c>
+      <c r="I6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr"/>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>73313581294534868820</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>65592250285068942839</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>Period event2</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>My first event period modify2</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
         <is>
           <t>2023-08-01 10:00:00</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
+      <c r="G7" t="inlineStr">
         <is>
           <t>2024-10-31 10:00:00</t>
         </is>
       </c>
-      <c r="G4" t="b">
+      <c r="H7" t="b">
         <v>1</v>
       </c>
-      <c r="H4" t="b">
+      <c r="I7" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>